<commit_message>
create time sheet and new ideas or knowledge
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcarr/Documents/CV_OrigamiRobot_Fall2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FAE325-7386-1C45-992A-D5E5B68B8113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198E1A93-D45D-444F-8986-228BAF1221E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3020" yWindow="2360" windowWidth="15500" windowHeight="16240" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,62 +502,69 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>45624</v>
+        <v>45563</v>
       </c>
       <c r="B2" s="3">
-        <v>0.125</v>
+        <v>0.625</v>
       </c>
       <c r="C2" s="3">
-        <v>0.20833333333333334</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D2" s="3">
         <f>C2-B2</f>
-        <v>8.3333333333333343E-2</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="E2" s="5">
         <f>D2*1440</f>
-        <v>120.00000000000001</v>
+        <v>120.00000000000006</v>
       </c>
       <c r="F2" s="5">
         <f>E2/60</f>
-        <v>2.0000000000000004</v>
+        <v>2.0000000000000009</v>
       </c>
       <c r="G2" s="7">
         <f>F2*22.5</f>
-        <v>45.000000000000007</v>
+        <v>45.000000000000021</v>
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>2.0000000000000004</v>
+        <v>3.5000000000000009</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>45.000000000000007</v>
+        <v>78.750000000000028</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>36.900000000000006</v>
+        <v>64.575000000000031</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="2">
+        <f ca="1">TODAY()</f>
+        <v>45565</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D3" s="3">
         <f>C3-B3</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E3" s="5">
         <f>D3*1440</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="F3" s="5">
         <f>E3/60</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G3" s="7">
         <f t="shared" ref="G3:G19" si="0">F3*22.5</f>
-        <v>0</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add cv_test.py and update
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcarr/Documents/CV_OrigamiRobot_Fall2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B56662-0BE2-934A-8097-02B1262580F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BC0819-C6C6-4A0A-81ED-B1659F8B9A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="2360" windowWidth="15500" windowHeight="16240" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,17 +461,17 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45563</v>
       </c>
@@ -531,20 +531,19 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>3.5000000000000009</v>
+        <v>-12</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>78.750000000000028</v>
+        <v>-270</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>64.575000000000031</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-221.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f ca="1">TODAY()</f>
         <v>45565</v>
       </c>
       <c r="B3" s="3">
@@ -570,28 +569,33 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f>A3</f>
+        <v>45565</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3">
         <f>C4-B4</f>
-        <v>0</v>
+        <v>-0.64583333333333337</v>
       </c>
       <c r="E4" s="5">
         <f>D4*1440</f>
-        <v>0</v>
+        <v>-930</v>
       </c>
       <c r="F4" s="5">
         <f>E4/60</f>
-        <v>0</v>
+        <v>-15.5</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-348.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -612,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -633,7 +637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -654,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -675,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -696,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -717,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -738,7 +742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -759,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -780,7 +784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -801,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -822,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -843,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -861,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D18" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -879,7 +883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D19" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -897,12 +901,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating time_sheet and update detection test
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83ED7DC-393A-4D31-8109-803B3C68D4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46CB4E4-B4F1-4819-801A-D8D2FCFD630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -531,15 +531,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>5.916666666666667</v>
+        <v>6.9166666666666661</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>133.125</v>
+        <v>155.62499999999997</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>109.16250000000001</v>
+        <v>127.61249999999998</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -598,24 +598,30 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="A5" s="2">
+        <v>45565</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
       <c r="D5" s="3">
         <f t="shared" ref="D5:D19" si="1">C5-B5</f>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:E19" si="2">D5*1440</f>
-        <v>0</v>
+        <v>59.999999999999943</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ref="F5:F19" si="3">E5/60</f>
-        <v>0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.499999999999979</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add transfer learning stuff
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcarr/Documents/CV_OrigamiRobot_Fall2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E9D469-B685-480B-8DAD-E6C3C116B665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13888642-E5C8-1E43-9C0D-5D3AF3A682A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,17 +467,17 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45563</v>
       </c>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>11.750000000000002</v>
+        <v>13.216666666666665</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>264.37500000000006</v>
+        <v>297.375</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>216.78750000000005</v>
+        <v>243.84750000000003</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -564,7 +564,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45565</v>
       </c>
@@ -603,7 +603,7 @@
         <v>219.37500000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f>A3</f>
         <v>45565</v>
@@ -634,8 +634,16 @@
         <f t="shared" ref="L4:L12" si="1">L3+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="3">
+        <f>SUM(D10:D11)</f>
+        <v>6.1111111111111005E-2</v>
+      </c>
+      <c r="N4" s="7">
+        <f>SUM(G10:G11)</f>
+        <v>32.999999999999943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45565</v>
       </c>
@@ -666,7 +674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45566</v>
       </c>
@@ -697,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45567</v>
       </c>
@@ -728,7 +736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45570</v>
       </c>
@@ -759,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45571</v>
       </c>
@@ -790,57 +798,69 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>45575</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.79027777777777775</v>
+      </c>
       <c r="D10" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.9444444444444375E-2</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27.999999999999901</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.46666666666666501</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.499999999999963</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>45575</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.875</v>
+      </c>
       <c r="D11" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>59.999999999999943</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.499999999999979</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -865,7 +885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -886,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -907,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -928,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -949,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D17" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -967,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D18" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -985,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1003,12 +1023,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying roboflow and training v8 model
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcarr/Documents/CV_OrigamiRobot_Fall2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FDF397-2C23-DF45-8962-4B2B707EA994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C2A95-423D-432F-9623-42D7782FD478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
+    <workbookView xWindow="-25275" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,17 +467,17 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45563</v>
       </c>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>13.833333333333332</v>
+        <v>15.899999999999999</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>311.25</v>
+        <v>357.75</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>255.22500000000002</v>
+        <v>293.35500000000002</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -563,8 +563,12 @@
         <f>D2</f>
         <v>8.333333333333337E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N2" s="7">
+        <f>G2</f>
+        <v>45.000000000000021</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45565</v>
       </c>
@@ -603,7 +607,7 @@
         <v>219.37500000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3</f>
         <v>45565</v>
@@ -635,15 +639,15 @@
         <v>3</v>
       </c>
       <c r="M4" s="3">
-        <f>SUM(D10:D11)</f>
-        <v>6.1111111111111005E-2</v>
+        <f>SUM(D10:D13)</f>
+        <v>0.17291666666666655</v>
       </c>
       <c r="N4" s="7">
-        <f>SUM(G10:G11)</f>
-        <v>32.999999999999943</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <f>SUM(G10:G13)</f>
+        <v>93.374999999999943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45565</v>
       </c>
@@ -674,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45566</v>
       </c>
@@ -705,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45567</v>
       </c>
@@ -736,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45570</v>
       </c>
@@ -767,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45571</v>
       </c>
@@ -798,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45575</v>
       </c>
@@ -829,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>45575</v>
       </c>
@@ -860,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45576</v>
       </c>
@@ -891,28 +895,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45577</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.57152777777777775</v>
+      </c>
       <c r="D13" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.6111111111111083E-2</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>123.99999999999996</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.066666666666666</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>46.499999999999986</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -933,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -954,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -975,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -993,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D18" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1011,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1029,12 +1039,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new training data, works for specific object detection
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apcarr\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C2A95-423D-432F-9623-42D7782FD478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D8F95E-BFCC-463D-BD9F-0602F24D5424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25275" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
+    <workbookView xWindow="3180" yWindow="3600" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -466,18 +466,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="2">
         <v>45563</v>
       </c>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>15.899999999999999</v>
+        <v>18.449999999999996</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>357.75</v>
+        <v>415.125</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>293.35500000000002</v>
+        <v>340.40250000000003</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -568,7 +568,7 @@
         <v>45.000000000000021</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="2">
         <v>45565</v>
       </c>
@@ -607,7 +607,7 @@
         <v>219.37500000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="2">
         <f>A3</f>
         <v>45565</v>
@@ -639,15 +639,15 @@
         <v>3</v>
       </c>
       <c r="M4" s="3">
-        <f>SUM(D10:D13)</f>
-        <v>0.17291666666666655</v>
+        <f>SUM(D10:D14)</f>
+        <v>0.27916666666666651</v>
       </c>
       <c r="N4" s="7">
-        <f>SUM(G10:G13)</f>
-        <v>93.374999999999943</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <f>SUM(G10:G14)</f>
+        <v>150.74999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2">
         <v>45565</v>
       </c>
@@ -678,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="2">
         <v>45566</v>
       </c>
@@ -709,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>45567</v>
       </c>
@@ -740,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>45570</v>
       </c>
@@ -771,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>45571</v>
       </c>
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>45575</v>
       </c>
@@ -833,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="8">
         <v>45575</v>
       </c>
@@ -864,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="2">
         <v>45576</v>
       </c>
@@ -895,7 +895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="2">
         <v>45577</v>
       </c>
@@ -922,28 +922,34 @@
         <v>46.499999999999986</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+    <row r="14" spans="1:14">
+      <c r="A14" s="8">
+        <v>45577</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.73333333333333328</v>
+      </c>
       <c r="D14" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.10624999999999996</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>152.99999999999994</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.5499999999999989</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>57.374999999999979</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -964,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -985,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="D17" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1003,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="D18" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1021,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7">
       <c r="D19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1039,12 +1045,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="15.75">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7">
       <c r="D31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cad, new friction idea
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apcarr\CV_OrigamiRobot_Fall2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D8F95E-BFCC-463D-BD9F-0602F24D5424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC85A273-5689-4EE9-9F10-39A9F7353B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3600" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
+    <workbookView xWindow="-25275" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -466,18 +466,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45563</v>
       </c>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>18.449999999999996</v>
+        <v>8.3166666666666629</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>415.125</v>
+        <v>187.125</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>340.40250000000003</v>
+        <v>153.44250000000002</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -568,7 +568,7 @@
         <v>45.000000000000021</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45565</v>
       </c>
@@ -607,7 +607,7 @@
         <v>219.37500000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3</f>
         <v>45565</v>
@@ -647,7 +647,7 @@
         <v>150.74999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45565</v>
       </c>
@@ -678,7 +678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45566</v>
       </c>
@@ -709,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45567</v>
       </c>
@@ -740,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45570</v>
       </c>
@@ -771,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45571</v>
       </c>
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45575</v>
       </c>
@@ -833,7 +833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>45575</v>
       </c>
@@ -864,7 +864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45576</v>
       </c>
@@ -895,7 +895,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45577</v>
       </c>
@@ -922,7 +922,7 @@
         <v>46.499999999999986</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>45577</v>
       </c>
@@ -949,28 +949,32 @@
         <v>57.374999999999979</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45578</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.42222222222222222</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.42222222222222222</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-608</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-10.133333333333333</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>-228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -991,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1009,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D18" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1027,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1045,12 +1049,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="15.75">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add solidworks photo to log
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC85A273-5689-4EE9-9F10-39A9F7353B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5159182F-BFB4-4440-9F44-85951CFA9D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25275" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>8.3166666666666629</v>
+        <v>21.399999999999995</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>187.125</v>
+        <v>481.5</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>153.44250000000002</v>
+        <v>394.83000000000004</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -639,12 +639,12 @@
         <v>3</v>
       </c>
       <c r="M4" s="3">
-        <f>SUM(D10:D14)</f>
-        <v>0.27916666666666651</v>
+        <f>SUM(D10:D15)</f>
+        <v>0.40208333333333313</v>
       </c>
       <c r="N4" s="7">
-        <f>SUM(G10:G14)</f>
-        <v>150.74999999999991</v>
+        <f>SUM(G10:G15)</f>
+        <v>217.12499999999989</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -956,22 +956,24 @@
       <c r="B15" s="3">
         <v>0.42222222222222222</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3">
+        <v>0.54513888888888884</v>
+      </c>
       <c r="D15" s="3">
         <f t="shared" si="2"/>
-        <v>-0.42222222222222222</v>
+        <v>0.12291666666666662</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" si="3"/>
-        <v>-608</v>
+        <v>176.99999999999994</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="4"/>
-        <v>-10.133333333333333</v>
+        <v>2.9499999999999988</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="0"/>
-        <v>-228</v>
+        <v>66.374999999999972</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixing spacing on clamp
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5159182F-BFB4-4440-9F44-85951CFA9D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF53F30C-A93B-434A-ADD2-B2D0F7D16734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25275" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -546,15 +546,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>21.399999999999995</v>
+        <v>22.233333333333327</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>481.5</v>
+        <v>500.25</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>394.83000000000004</v>
+        <v>410.20500000000004</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -639,12 +639,12 @@
         <v>3</v>
       </c>
       <c r="M4" s="3">
-        <f>SUM(D10:D15)</f>
-        <v>0.40208333333333313</v>
+        <f>SUM(D10:D16)</f>
+        <v>0.43680555555555534</v>
       </c>
       <c r="N4" s="7">
-        <f>SUM(G10:G15)</f>
-        <v>217.12499999999989</v>
+        <f>SUM(G10:G16)</f>
+        <v>235.87499999999989</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -977,24 +977,30 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="2">
+        <v>45578</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.58611111111111114</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.62083333333333335</v>
+      </c>
       <c r="D16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>49.999999999999986</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.83333333333333315</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.749999999999996</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
friction pads and new clamp walls
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF53F30C-A93B-434A-ADD2-B2D0F7D16734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E07840-F0E8-4AF5-AE86-02950E3D2EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25275" yWindow="1320" windowWidth="21600" windowHeight="11295" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -120,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -130,6 +130,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,7 +468,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -546,15 +547,15 @@
       </c>
       <c r="H2" s="5">
         <f>SUM(F:F)</f>
-        <v>22.233333333333327</v>
+        <v>23.883333333333326</v>
       </c>
       <c r="I2" s="7">
         <f>SUM(G:G)</f>
-        <v>500.25</v>
+        <v>537.375</v>
       </c>
       <c r="J2" s="7">
         <f>I2*(1-0.18)</f>
-        <v>410.20500000000004</v>
+        <v>440.64750000000004</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -639,12 +640,12 @@
         <v>3</v>
       </c>
       <c r="M4" s="3">
-        <f>SUM(D10:D16)</f>
-        <v>0.43680555555555534</v>
+        <f>SUM(D10:D17)</f>
+        <v>0.50555555555555531</v>
       </c>
       <c r="N4" s="7">
-        <f>SUM(G10:G16)</f>
-        <v>235.87499999999989</v>
+        <f>SUM(G10:G17)</f>
+        <v>272.99999999999989</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1003,66 +1004,75 @@
         <v>18.749999999999996</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45578</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.91388888888888886</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.98263888888888884</v>
+      </c>
       <c r="D17" s="3">
         <f t="shared" si="2"/>
+        <v>6.8749999999999978E-2</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="3"/>
+        <v>98.999999999999972</v>
+      </c>
+      <c r="F17" s="5">
+        <f t="shared" si="4"/>
+        <v>1.6499999999999995</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>37.124999999999986</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E18" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F18" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G18" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F19" s="5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G19" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a whole bunch
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcarr/Documents/CV_OrigamiRobot_Fall2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1F2B52-9B39-E442-8C72-FB55DD2FC29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5BF714-8184-4F5C-9B07-F6337F7F243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,20 +471,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +528,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45563</v>
       </c>
@@ -559,15 +559,15 @@
       </c>
       <c r="I2" s="5">
         <f>SUM(F:F)</f>
-        <v>45.099999999999994</v>
+        <v>53.18333333333333</v>
       </c>
       <c r="J2" s="7">
         <f>SUM(G:G)</f>
-        <v>1014.75</v>
+        <v>1196.625</v>
       </c>
       <c r="K2" s="7">
         <f>J2*(1-0.18)</f>
-        <v>832.09500000000003</v>
+        <v>981.23250000000007</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -581,7 +581,7 @@
         <v>45.000000000000021</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45565</v>
       </c>
@@ -604,7 +604,7 @@
         <v>1.5</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G28" si="0">F3*22.5</f>
+        <f t="shared" ref="G3:G32" si="0">F3*22.5</f>
         <v>33.75</v>
       </c>
       <c r="H3" t="s">
@@ -623,7 +623,7 @@
         <v>219.37500000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3</f>
         <v>45565</v>
@@ -666,7 +666,7 @@
         <v>272.99999999999989</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45565</v>
       </c>
@@ -677,15 +677,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D28" si="2">C5-B5</f>
+        <f t="shared" ref="D5:D32" si="2">C5-B5</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E28" si="3">D5*1440</f>
+        <f t="shared" ref="E5:E32" si="3">D5*1440</f>
         <v>59.999999999999943</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F28" si="4">E5/60</f>
+        <f t="shared" ref="F5:F32" si="4">E5/60</f>
         <v>0.999999999999999</v>
       </c>
       <c r="G5" s="7">
@@ -708,7 +708,7 @@
         <v>220.87500000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45566</v>
       </c>
@@ -750,7 +750,7 @@
         <v>256.49999999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45567</v>
       </c>
@@ -783,8 +783,16 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M7" s="3">
+        <f>SUM(D29:D32)</f>
+        <v>0.33680555555555552</v>
+      </c>
+      <c r="N7" s="7">
+        <f>SUM(G29:G32)</f>
+        <v>181.87499999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45570</v>
       </c>
@@ -818,7 +826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45571</v>
       </c>
@@ -852,7 +860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45575</v>
       </c>
@@ -886,7 +894,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>45575</v>
       </c>
@@ -920,7 +928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45576</v>
       </c>
@@ -954,7 +962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45577</v>
       </c>
@@ -984,7 +992,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>45577</v>
       </c>
@@ -1014,7 +1022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45578</v>
       </c>
@@ -1044,7 +1052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45578</v>
       </c>
@@ -1074,7 +1082,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45578</v>
       </c>
@@ -1104,7 +1112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45579</v>
       </c>
@@ -1134,7 +1142,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45580</v>
       </c>
@@ -1164,7 +1172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45583</v>
       </c>
@@ -1194,7 +1202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45584</v>
       </c>
@@ -1224,7 +1232,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45585</v>
       </c>
@@ -1254,7 +1262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45586</v>
       </c>
@@ -1284,7 +1292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45588</v>
       </c>
@@ -1314,7 +1322,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45588</v>
       </c>
@@ -1344,7 +1352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45592</v>
       </c>
@@ -1374,7 +1382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45592</v>
       </c>
@@ -1404,7 +1412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45592</v>
       </c>
@@ -1434,11 +1442,116 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D31" s="3"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>45598</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="2"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="3"/>
+        <v>104.99999999999994</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7499999999999991</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="0"/>
+        <v>39.374999999999979</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>45598</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="2"/>
+        <v>3.0555555555555558E-2</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="4"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0.59375</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="2"/>
+        <v>0.17638888888888887</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="3"/>
+        <v>253.99999999999997</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="4"/>
+        <v>4.2333333333333325</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="0"/>
+        <v>95.249999999999986</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45600</v>
+      </c>
+      <c r="B32" s="9">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0.87291666666666667</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="2"/>
+        <v>5.6944444444444464E-2</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="3"/>
+        <v>82.000000000000028</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="4"/>
+        <v>1.3666666666666671</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="0"/>
+        <v>30.750000000000011</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create new friction pads
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53097E5B-91C7-4B6E-90B0-B5A279735287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D904311-B64E-4CFB-9549-4BB907FDE1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="840" windowWidth="25560" windowHeight="14430" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,15 +559,15 @@
       </c>
       <c r="I2" s="5">
         <f>SUM(F:F)</f>
-        <v>53.783333333333331</v>
+        <v>54.949999999999996</v>
       </c>
       <c r="J2" s="7">
         <f>SUM(G:G)</f>
-        <v>1210.125</v>
+        <v>1236.375</v>
       </c>
       <c r="K2" s="7">
         <f>J2*(1-0.18)</f>
-        <v>992.30250000000012</v>
+        <v>1013.8275000000001</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>1.5</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G33" si="0">F3*22.5</f>
+        <f t="shared" ref="G3:G34" si="0">F3*22.5</f>
         <v>33.75</v>
       </c>
       <c r="H3" t="s">
@@ -677,15 +677,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D33" si="2">C5-B5</f>
+        <f t="shared" ref="D5:D34" si="2">C5-B5</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E33" si="3">D5*1440</f>
+        <f t="shared" ref="E5:E34" si="3">D5*1440</f>
         <v>59.999999999999943</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F33" si="4">E5/60</f>
+        <f t="shared" ref="F5:F34" si="4">E5/60</f>
         <v>0.999999999999999</v>
       </c>
       <c r="G5" s="7">
@@ -825,6 +825,14 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
+      <c r="M8" s="3">
+        <f>SUM(D34)</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="N8" s="7">
+        <f>SUM(G34)</f>
+        <v>26.249999999999968</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1498,7 +1506,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>45600</v>
+        <v>45599</v>
       </c>
       <c r="B31" s="9">
         <v>0.41736111111111113</v>
@@ -1525,7 +1533,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>45600</v>
+        <v>45599</v>
       </c>
       <c r="B32" s="9">
         <v>0.81597222222222221</v>
@@ -1552,7 +1560,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>45600</v>
+        <v>45599</v>
       </c>
       <c r="B33" s="9">
         <v>0.94444444444444442</v>
@@ -1577,8 +1585,35 @@
         <v>13.500000000000009</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>45601</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="2"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="3"/>
+        <v>69.999999999999915</v>
+      </c>
+      <c r="F34" s="5">
+        <f t="shared" si="4"/>
+        <v>1.1666666666666652</v>
+      </c>
+      <c r="G34" s="7">
+        <f t="shared" si="0"/>
+        <v>26.249999999999968</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new friction pad
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC38795-9FB0-4BC4-A79D-85451B10E0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698D0528-7AA0-4509-B007-E73CB6858158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="840" windowWidth="25560" windowHeight="14430" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,15 +559,15 @@
       </c>
       <c r="I2" s="5">
         <f>SUM(F:F)</f>
-        <v>57.833333333333329</v>
+        <v>60.11666666666666</v>
       </c>
       <c r="J2" s="7">
         <f>SUM(G:G)</f>
-        <v>1301.25</v>
+        <v>1352.625</v>
       </c>
       <c r="K2" s="7">
         <f>J2*(1-0.18)</f>
-        <v>1067.0250000000001</v>
+        <v>1109.1525000000001</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>1.5</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G36" si="0">F3*22.5</f>
+        <f t="shared" ref="G3:G39" si="0">F3*22.5</f>
         <v>33.75</v>
       </c>
       <c r="H3" t="s">
@@ -677,15 +677,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D36" si="2">C5-B5</f>
+        <f t="shared" ref="D5:D39" si="2">C5-B5</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E36" si="3">D5*1440</f>
+        <f t="shared" ref="E5:E39" si="3">D5*1440</f>
         <v>59.999999999999943</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F36" si="4">E5/60</f>
+        <f t="shared" ref="F5:F39" si="4">E5/60</f>
         <v>0.999999999999999</v>
       </c>
       <c r="G5" s="7">
@@ -826,12 +826,12 @@
         <v>7</v>
       </c>
       <c r="M8" s="3">
-        <f>SUM(D34:D36)</f>
-        <v>0.16874999999999996</v>
+        <f>SUM(D34:D39)</f>
+        <v>0.26388888888888895</v>
       </c>
       <c r="N8" s="7">
-        <f>SUM(G34:G36)</f>
-        <v>91.124999999999972</v>
+        <f>SUM(G34:G39)</f>
+        <v>142.50000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1664,6 +1664,87 @@
       <c r="G36" s="7">
         <f t="shared" si="0"/>
         <v>17.999999999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>45603</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.75694444444444442</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="3"/>
+        <v>60.000000000000107</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="4"/>
+        <v>1.0000000000000018</v>
+      </c>
+      <c r="G37" s="7">
+        <f t="shared" si="0"/>
+        <v>22.500000000000039</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>45603</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.89930555555555558</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="2"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="3"/>
+        <v>40.000000000000014</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="4"/>
+        <v>0.66666666666666685</v>
+      </c>
+      <c r="G38" s="7">
+        <f t="shared" si="0"/>
+        <v>15.000000000000004</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>45604</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.54513888888888884</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="2"/>
+        <v>2.5694444444444464E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="3"/>
+        <v>37.000000000000028</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="4"/>
+        <v>0.61666666666666714</v>
+      </c>
+      <c r="G39" s="7">
+        <f t="shared" si="0"/>
+        <v>13.875000000000011</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
create dc control script
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6620D596-411B-4D3C-9669-4CD9A5318F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB371377-4571-47C0-A782-E901A0C41261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="795" yWindow="1050" windowWidth="25560" windowHeight="14430" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,15 +559,15 @@
       </c>
       <c r="I2" s="5">
         <f>SUM(F:F)</f>
-        <v>64.199999999999989</v>
+        <v>67.916666666666657</v>
       </c>
       <c r="J2" s="7">
         <f>SUM(G:G)</f>
-        <v>1444.5</v>
+        <v>1528.125</v>
       </c>
       <c r="K2" s="7">
         <f>J2*(1-0.18)</f>
-        <v>1184.49</v>
+        <v>1253.0625</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>1.5</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G41" si="0">F3*22.5</f>
+        <f t="shared" ref="G3:G42" si="0">F3*22.5</f>
         <v>33.75</v>
       </c>
       <c r="H3" t="s">
@@ -677,15 +677,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D41" si="2">C5-B5</f>
+        <f t="shared" ref="D5:D42" si="2">C5-B5</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E41" si="3">D5*1440</f>
+        <f t="shared" ref="E5:E42" si="3">D5*1440</f>
         <v>59.999999999999943</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F41" si="4">E5/60</f>
+        <f t="shared" ref="F5:F42" si="4">E5/60</f>
         <v>0.999999999999999</v>
       </c>
       <c r="G5" s="7">
@@ -1799,6 +1799,41 @@
       <c r="G41" s="7">
         <f t="shared" si="0"/>
         <v>48.000000000000007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>45607</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="2"/>
+        <v>0.15486111111111117</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="3"/>
+        <v>223.00000000000009</v>
+      </c>
+      <c r="F42" s="5">
+        <f t="shared" si="4"/>
+        <v>3.7166666666666681</v>
+      </c>
+      <c r="G42" s="7">
+        <f t="shared" si="0"/>
+        <v>83.625000000000028</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>45607</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0.62986111111111109</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add log entry and update time
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB371377-4571-47C0-A782-E901A0C41261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B53FB-78ED-44A0-8BE9-4E5FFC364F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="795" yWindow="1050" windowWidth="25560" windowHeight="14430" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -474,7 +474,7 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -559,15 +559,15 @@
       </c>
       <c r="I2" s="5">
         <f>SUM(F:F)</f>
-        <v>67.916666666666657</v>
+        <v>71.166666666666657</v>
       </c>
       <c r="J2" s="7">
         <f>SUM(G:G)</f>
-        <v>1528.125</v>
+        <v>1601.25</v>
       </c>
       <c r="K2" s="7">
         <f>J2*(1-0.18)</f>
-        <v>1253.0625</v>
+        <v>1313.0250000000001</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -604,7 +604,7 @@
         <v>1.5</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G42" si="0">F3*22.5</f>
+        <f t="shared" ref="G3:G43" si="0">F3*22.5</f>
         <v>33.75</v>
       </c>
       <c r="H3" t="s">
@@ -677,15 +677,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D42" si="2">C5-B5</f>
+        <f t="shared" ref="D5:D43" si="2">C5-B5</f>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" ref="E5:E42" si="3">D5*1440</f>
+        <f t="shared" ref="E5:E43" si="3">D5*1440</f>
         <v>59.999999999999943</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" ref="F5:F42" si="4">E5/60</f>
+        <f t="shared" ref="F5:F43" si="4">E5/60</f>
         <v>0.999999999999999</v>
       </c>
       <c r="G5" s="7">
@@ -867,6 +867,14 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="M9" s="3">
+        <f xml:space="preserve"> SUM(D42:D43)</f>
+        <v>0.2902777777777778</v>
+      </c>
+      <c r="N9" s="7">
+        <f xml:space="preserve"> SUM(G42:G43)</f>
+        <v>156.75</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1834,6 +1842,25 @@
       </c>
       <c r="B43" s="9">
         <v>0.62986111111111109</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.76527777777777772</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="2"/>
+        <v>0.13541666666666663</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="3"/>
+        <v>194.99999999999994</v>
+      </c>
+      <c r="F43" s="5">
+        <f t="shared" si="4"/>
+        <v>3.2499999999999991</v>
+      </c>
+      <c r="G43" s="7">
+        <f t="shared" si="0"/>
+        <v>73.124999999999986</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add script to pos pid
</commit_message>
<xml_diff>
--- a/Excel Time Sheet.xlsx
+++ b/Excel Time Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Carr\Downloads\CV_OrigamiRobot_Fall2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909B53FB-78ED-44A0-8BE9-4E5FFC364F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B228D57-FF45-4555-8770-B344C7535CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="795" yWindow="1050" windowWidth="25560" windowHeight="14430" xr2:uid="{224015C0-04A6-AE4F-9153-85C745022AD7}"/>
   </bookViews>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6450EA8C-00B7-4644-8B52-A8FB020FE4FD}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1863,8 +1863,16 @@
         <v>73.124999999999986</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>45608</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0.85277777777777775</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>